<commit_message>
Added calculations to the TasksDone sheet
</commit_message>
<xml_diff>
--- a/Docs/Statistics.xlsx
+++ b/Docs/Statistics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Time Overview" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="TasksDone" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TasksDone!$A$1:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TasksDone!$A$1:$F$3</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Pacman</t>
   </si>
@@ -160,13 +160,16 @@
   </si>
   <si>
     <t>WBS</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,32 +233,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -270,6 +290,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -303,7 +324,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4.5</c:v>
@@ -332,6 +353,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -394,6 +416,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -456,6 +479,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -518,6 +542,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -580,6 +605,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -642,6 +668,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -704,6 +731,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>WorkDone!$A$4:$A$8</c:f>
@@ -752,34 +780,50 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="235322368"/>
-        <c:axId val="235691392"/>
+        <c:axId val="97524736"/>
+        <c:axId val="97551104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235322368"/>
+        <c:axId val="97524736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235691392"/>
+        <c:crossAx val="97551104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235691392"/>
+        <c:axId val="97551104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235322368"/>
+        <c:crossAx val="97524736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -787,9 +831,234 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="sv-SE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Estimated Hours</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TasksDone!$A$3:$B$9</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="7"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Total</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Set up templates</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>WBS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Meetings</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Architecture diagrams</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Weekly Reports</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>High Design Report</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>L1: High design</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TasksDone!$D$3:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Actual Hours</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TasksDone!$A$3:$B$9</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="7"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Total</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Set up templates</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>WBS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Meetings</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Architecture diagrams</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Weekly Reports</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>High Design Report</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>L1: High design</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TasksDone!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="99665792"/>
+        <c:axId val="99667328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="99665792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99667328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="99667328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="99665792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -834,8 +1103,207 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="textruta 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7467600" y="304799"/>
+          <a:ext cx="4076700" cy="2009775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>OBS!</a:t>
+          </a:r>
+          <a:endParaRPr lang="sv-SE" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>När</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> ni vill infoga en ny rad (genom att markera en rad, högerklicka och välja </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" i="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Infoga</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>), välj då </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>inte</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> raden precis under rubriken (L1, L2, L3 och L4). Det gör att formlerna uppdaterar sig fel och första raden kommer då inte att räknas med. Det är på grund av detta som jag har lagt in två tomma rader mellan varje rubrik.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100" b="0" i="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Dvs, för att infoga en rad, markera raden två rader (eller mer) under rubriken, ex. rad 5 för att infoga under L1, och välj sedan infoga.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100" b="0" i="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="sv-SE" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Exempel på hur grafen kan se ut ser ni nedan:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="sv-SE" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Diagram 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -909,6 +1377,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -943,6 +1412,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1118,79 +1588,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="46.5">
+    <row r="1" spans="1:1" ht="46.5" x14ac:dyDescent="0.7">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1202,64 +1672,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="9" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="6" customFormat="1">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1288,12 +1758,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1317,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1346,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1375,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1404,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1"/>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
@@ -1415,37 +1885,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1456,106 +1924,182 @@
         <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <f>SUM(D4:INDEX(D4:D1004,MATCH(TRUE,INDEX(D4:D1004="",0),0)))</f>
+        <v>10.5</v>
+      </c>
+      <c r="E3">
+        <f>SUM(E4:INDEX(E4:E1004,MATCH(TRUE,INDEX(E4:E1004="",0),0)))</f>
+        <v>3.5</v>
+      </c>
+      <c r="F3">
+        <f>COUNTA(B4:INDEX(B4:B1004,MATCH(TRUE,INDEX(B4:B1004="",0),0)))</f>
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <f>COUNTA(C4:INDEX(C4:C1004,MATCH(TRUE,INDEX(C4:C1004="",0),0)))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>45</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="E4">
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>46</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="D5">
         <v>0.5</v>
       </c>
-      <c r="G5">
+      <c r="E5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>41</v>
       </c>
-      <c r="F6">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="G6">
+      <c r="E6">
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="F7">
+      <c r="D7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>42</v>
       </c>
-      <c r="F8">
+      <c r="D8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="F9">
+      <c r="D9">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <f>SUM(D12:INDEX(D12:D1012,MATCH(TRUE,INDEX(D12:D1012="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E12:INDEX(E12:E1012,MATCH(TRUE,INDEX(E12:E1012="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <f>COUNTA(B12:INDEX(B12:B1012,MATCH(TRUE,INDEX(B12:B1012="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f>COUNTA(C12:INDEX(C12:C1012,MATCH(TRUE,INDEX(C12:C1012="",0),0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
+        <f>SUM(D15:INDEX(D15:D1015,MATCH(TRUE,INDEX(D15:D1015="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f>SUM(E15:INDEX(E15:E1015,MATCH(TRUE,INDEX(E15:E1015="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>COUNTA(B15:INDEX(B15:B1015,MATCH(TRUE,INDEX(B15:B1015="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f>COUNTA(C15:INDEX(C15:C1015,MATCH(TRUE,INDEX(C15:C1015="",0),0)))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17">
+        <f>SUM(D18:INDEX(D18:D1018,MATCH(TRUE,INDEX(D18:D1018="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>SUM(E18:INDEX(E18:E1018,MATCH(TRUE,INDEX(E18:E1018="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>COUNTA(B18:INDEX(B18:B1018,MATCH(TRUE,INDEX(B18:B1018="",0),0)))</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>COUNTA(C18:INDEX(C18:C1018,MATCH(TRUE,INDEX(C18:C1018="",0),0)))</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>